<commit_message>
Deploying to gh-pages from @ eurovibes/dreh_shield@ddd7d17db12d1d3c62c75617f01a7b7efe5b7392 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/dreh_shield-bom_0.1.xlsx
+++ b/Fabrication/BoM/dreh_shield-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="102">
   <si>
     <t>Row</t>
   </si>
@@ -116,6 +116,15 @@
     <t>AB1</t>
   </si>
   <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>2946-236-402-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/wago-corporation/236-402/15573417</t>
+  </si>
+  <si>
     <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
   </si>
   <si>
@@ -131,6 +140,12 @@
     <t>Analog</t>
   </si>
   <si>
+    <t>SAM9298-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/samtec-inc/ESQ-106-14-T-S/6678035</t>
+  </si>
+  <si>
     <t>PinSocket_1x06_P2.54mm_Vertical</t>
   </si>
   <si>
@@ -149,6 +164,12 @@
     <t>Digital/PWM</t>
   </si>
   <si>
+    <t>SAM15577-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/samtec-inc/ESQ-110-14-T-S/6692348</t>
+  </si>
+  <si>
     <t>PinSocket_1x10_P2.54mm_Vertical</t>
   </si>
   <si>
@@ -165,6 +186,12 @@
   </si>
   <si>
     <t>Power</t>
+  </si>
+  <si>
+    <t>SAM9303-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/samtec-inc/ESQ-108-14-T-S/6678040</t>
   </si>
   <si>
     <t>PinSocket_1x08_P2.54mm_Vertical</t>
@@ -799,7 +826,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -813,13 +840,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F2" s="3">
         <v>10</v>
@@ -827,13 +854,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="F3" s="3">
         <v>25</v>
@@ -841,13 +868,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="F4" s="3">
         <v>25</v>
@@ -855,13 +882,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -869,13 +896,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F6" s="3">
         <v>25</v>
@@ -1015,19 +1042,19 @@
         <v>16</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>28</v>
@@ -1038,13 +1065,13 @@
         <v>21</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>16</v>
@@ -1053,19 +1080,19 @@
         <v>16</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>12</v>
@@ -1073,16 +1100,16 @@
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>16</v>
@@ -1091,19 +1118,19 @@
         <v>16</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>12</v>
@@ -1111,16 +1138,16 @@
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>16</v>
@@ -1129,19 +1156,19 @@
         <v>16</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>22</v>
@@ -1149,16 +1176,16 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="5" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>16</v>
@@ -1176,7 +1203,7 @@
         <v>16</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>16</v>
@@ -1187,16 +1214,16 @@
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>16</v>
@@ -1211,30 +1238,30 @@
         <v>16</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="K16" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>16</v>
@@ -1249,13 +1276,13 @@
         <v>16</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>12</v>
@@ -1263,16 +1290,16 @@
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>16</v>
@@ -1287,13 +1314,13 @@
         <v>16</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>12</v>
@@ -1334,22 +1361,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>